<commit_message>
Correção de datas dos eventos nos documentos
</commit_message>
<xml_diff>
--- a/src/docs/calendario-corridas26.xlsx
+++ b/src/docs/calendario-corridas26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ccpagencia/Desktop/TEMP/motorsport26.json/calendario-corridas2026/src/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C8CD03-A694-034B-8D50-E72F0CD08DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAF336D-9F81-E346-95C0-A21F2C2CB6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="2540" windowWidth="37560" windowHeight="22340" xr2:uid="{F700CC5D-BB2C-554E-9C80-469F0288F0F2}"/>
+    <workbookView xWindow="15180" yWindow="2540" windowWidth="34100" windowHeight="22340" xr2:uid="{F700CC5D-BB2C-554E-9C80-469F0288F0F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="173">
   <si>
     <t>Rolex 24 At Daytona</t>
   </si>
@@ -552,12 +552,21 @@
   </si>
   <si>
     <t>06 de dezembro</t>
+  </si>
+  <si>
+    <t>29 de novembro</t>
+  </si>
+  <si>
+    <t>22 de novembro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$]hh:mm;@" x16r2:formatCode16="[$-en-BR,1]hh:mm;@"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -661,7 +670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -705,13 +714,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -720,16 +723,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -741,9 +742,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFABC2DE"/>
+      <color rgb="FF8DB5DF"/>
+      <color rgb="FF00A3E0"/>
       <color rgb="FFFFE5E6"/>
       <color rgb="FFFFB5AD"/>
-      <color rgb="FF00A3E0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -755,6 +758,1691 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1068" name="AutoShape 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A105BE6-161D-69FE-E8F7-B05D443967E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="1066800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1069" name="AutoShape 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090F69B5-114C-901D-9403-D670521C3148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="1473200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1070" name="AutoShape 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D60178BE-4763-E5FA-CF3F-87E5AFABE7A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="1879600"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1071" name="AutoShape 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D07B898A-E08F-A73E-1AA9-D140B2F6AE5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="2286000"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1073" name="AutoShape 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0485140-C6F8-DAB6-6AE4-6E92372433BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="3098800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1074" name="AutoShape 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8AD2496-6A69-F6C9-8979-593B4BB16FEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="3505200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1075" name="AutoShape 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1902DA25-A2FA-E3B2-47A9-D46784F3EA88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="3911600"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1077" name="AutoShape 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64D50903-1777-91DA-8CFD-14264D47351D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="4724400"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1078" name="AutoShape 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1197B46E-C560-C145-4DB7-1178F866C0E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="5130800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1079" name="AutoShape 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6815CF24-4BCD-DFE0-6399-E2022F8C3326}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="5537200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1081" name="AutoShape 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA615714-9CAA-B2DB-BF49-6CADD29101BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="6350000"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1082" name="AutoShape 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC6E16FB-12BF-F827-D89B-CF3F15C6FDCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="6756400"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1083" name="AutoShape 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08A79C11-74EC-BEC0-AE69-1152C7443F96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="7162800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1084" name="AutoShape 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0F8674-D495-A29A-3E8A-E3C673125522}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="7569200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1086" name="AutoShape 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E7D5B5D-915D-7A12-9FE7-4B568BC152AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="8382000"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1087" name="AutoShape 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E9AA484-F067-9E23-1FA5-7308FAE99336}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="8788400"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1088" name="AutoShape 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB4983D8-D10B-2DF4-FD32-700193D1BB9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="9194800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1089" name="AutoShape 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B865C69-0059-C713-4972-F5F26D642B89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="9601200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1091" name="AutoShape 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F22082D4-5716-C7F5-6BB3-46F8F25FC86F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="10414000"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1092" name="AutoShape 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE27E39F-41E4-B7AC-0BDB-AF69B306E7C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="10820400"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1093" name="AutoShape 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6FB344F-F500-3224-2C56-6E16F3B59DED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="11226800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1094" name="AutoShape 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64CC1FA0-A29B-1EBC-ADA3-4D958EA56B0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="11633200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1095" name="AutoShape 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{126E89AF-54AB-A34B-6FB2-3738FD942EA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="12039600"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1096" name="AutoShape 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E838BBED-3699-BFD5-8425-E8593C9F672C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="12446000"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1098" name="AutoShape 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1907A173-5785-4051-211D-4A15F232DC59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="13258800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1099" name="AutoShape 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49954CC1-1D63-8739-D6A6-2E842149ED3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="13665200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1100" name="AutoShape 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0FCC09C-28AD-3B5E-47C4-49A033050BEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="14071600"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1102" name="AutoShape 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5F37271-BA57-5984-C85F-F25F4571348C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="14884400"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1103" name="AutoShape 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF0ACE59-BE60-65F6-C12F-71ACFBB5E96A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="15290800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1104" name="AutoShape 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C05285F-01E9-F5B4-AD1C-72B7BB5E09D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="15697200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1105" name="AutoShape 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42D9BBF1-ED65-7821-97A3-F9FCFDB4FFB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="16103600"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1106" name="AutoShape 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD9EA727-6BBF-820C-8897-96AC2D4FBD06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="16510000"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1108" name="AutoShape 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1425B43-954C-D375-2CAC-34E4ACC68BC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="17322800"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>355600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1109" name="AutoShape 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C02612A6-F1CD-B4D4-6839-392327E3668A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="17729200"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1110" name="AutoShape 86">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CB7464D-C9C9-BC11-51D7-2DA56FFD033D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="18135600"/>
+          <a:ext cx="762000" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1073,14 +2761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3B01EF-F7D4-C840-AA78-CF853344D978}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3B01EF-F7D4-C840-AA78-CF853344D978}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:H45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1089,9 +2777,9 @@
     <col min="3" max="3" width="45.28515625" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="6" max="6" width="18" style="18" customWidth="1"/>
     <col min="7" max="7" width="60.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13" style="15" customWidth="1"/>
+    <col min="8" max="8" width="13" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="30" customHeight="1"/>
@@ -1108,13 +2796,13 @@
       <c r="E2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="19" t="s">
         <v>89</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="16"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="2:8" ht="32" customHeight="1">
       <c r="B3" s="7" t="s">
@@ -1123,7 +2811,7 @@
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1135,7 +2823,7 @@
       <c r="G3" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="2:8" ht="32" customHeight="1">
       <c r="B4" s="13" t="s">
@@ -1144,7 +2832,7 @@
       <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1156,7 +2844,7 @@
       <c r="G4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="17"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:8" ht="32" customHeight="1">
       <c r="B5" s="14" t="s">
@@ -1165,7 +2853,7 @@
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1177,7 +2865,7 @@
       <c r="G5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="32" customHeight="1">
       <c r="B6" s="10" t="s">
@@ -1186,19 +2874,19 @@
       <c r="C6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="2:8" ht="32" customHeight="1">
       <c r="B7" s="11" t="s">
@@ -1207,19 +2895,19 @@
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="32" customHeight="1">
       <c r="B8" s="13" t="s">
@@ -1228,7 +2916,7 @@
       <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -1240,7 +2928,7 @@
       <c r="G8" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="17"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:8" ht="32" customHeight="1">
       <c r="B9" s="14" t="s">
@@ -1249,7 +2937,7 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1261,7 +2949,7 @@
       <c r="G9" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="17"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:8" ht="32" customHeight="1">
       <c r="B10" s="13" t="s">
@@ -1270,7 +2958,7 @@
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="8" t="s">
@@ -1282,7 +2970,7 @@
       <c r="G10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:8" ht="32" customHeight="1">
       <c r="B11" s="11" t="s">
@@ -1291,19 +2979,19 @@
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="17"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="32" customHeight="1">
       <c r="B12" s="10" t="s">
@@ -1312,19 +3000,19 @@
       <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="H12" s="17"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:8" ht="32" customHeight="1">
       <c r="B13" s="14" t="s">
@@ -1333,7 +3021,7 @@
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>21</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1345,7 +3033,7 @@
       <c r="G13" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="32" customHeight="1">
       <c r="B14" s="10" t="s">
@@ -1354,19 +3042,19 @@
       <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="H14" s="17"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:8" ht="32" customHeight="1">
       <c r="B15" s="11" t="s">
@@ -1375,19 +3063,19 @@
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:8" ht="32" customHeight="1">
       <c r="B16" s="13" t="s">
@@ -1396,7 +3084,7 @@
       <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1408,7 +3096,7 @@
       <c r="G16" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="17"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:8" ht="32" customHeight="1">
       <c r="B17" s="7" t="s">
@@ -1417,19 +3105,19 @@
       <c r="C17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="H17" s="17"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8" ht="32" customHeight="1">
       <c r="B18" s="13" t="s">
@@ -1438,7 +3126,7 @@
       <c r="C18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -1450,7 +3138,7 @@
       <c r="G18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="2:8" ht="32" customHeight="1">
       <c r="B19" s="14" t="s">
@@ -1459,7 +3147,7 @@
       <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1471,7 +3159,7 @@
       <c r="G19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" ht="32" customHeight="1">
       <c r="B20" s="12" t="s">
@@ -1480,19 +3168,19 @@
       <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="17"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="2:8" ht="32" customHeight="1">
       <c r="B21" s="14" t="s">
@@ -1501,7 +3189,7 @@
       <c r="C21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1513,7 +3201,7 @@
       <c r="G21" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="2:8" ht="32" customHeight="1">
       <c r="B22" s="10" t="s">
@@ -1522,19 +3210,19 @@
       <c r="C22" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="2:8" ht="32" customHeight="1">
       <c r="B23" s="14" t="s">
@@ -1543,7 +3231,7 @@
       <c r="C23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1555,7 +3243,7 @@
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="17"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8" ht="32" customHeight="1">
       <c r="B24" s="13" t="s">
@@ -1564,7 +3252,7 @@
       <c r="C24" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -1576,7 +3264,7 @@
       <c r="G24" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="17"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="2:8" ht="32" customHeight="1">
       <c r="B25" s="11" t="s">
@@ -1585,19 +3273,19 @@
       <c r="C25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="F25" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="17"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="2:8" ht="32" customHeight="1">
       <c r="B26" s="10" t="s">
@@ -1606,19 +3294,19 @@
       <c r="C26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="17" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="17"/>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:8" ht="32" customHeight="1">
       <c r="B27" s="14" t="s">
@@ -1627,7 +3315,7 @@
       <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>48</v>
       </c>
       <c r="E27" s="3" t="s">
@@ -1639,7 +3327,7 @@
       <c r="G27" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H27" s="17"/>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="2:8" ht="32" customHeight="1">
       <c r="B28" s="10" t="s">
@@ -1648,19 +3336,19 @@
       <c r="C28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="17" t="s">
         <v>50</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H28" s="17"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="2:8" ht="32" customHeight="1">
       <c r="B29" s="14" t="s">
@@ -1669,7 +3357,7 @@
       <c r="C29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1681,7 +3369,7 @@
       <c r="G29" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H29" s="17"/>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="2:8" ht="32" customHeight="1">
       <c r="B30" s="10" t="s">
@@ -1690,19 +3378,19 @@
       <c r="C30" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="17"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="2:8" ht="32" customHeight="1">
       <c r="B31" s="14" t="s">
@@ -1711,7 +3399,7 @@
       <c r="C31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="16" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
@@ -1723,7 +3411,7 @@
       <c r="G31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H31" s="17"/>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="2:8" ht="32" customHeight="1">
       <c r="B32" s="12" t="s">
@@ -1732,19 +3420,19 @@
       <c r="C32" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="17" t="s">
         <v>58</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H32" s="17"/>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="2:8" ht="32" customHeight="1">
       <c r="B33" s="14" t="s">
@@ -1753,7 +3441,7 @@
       <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="16" t="s">
         <v>60</v>
       </c>
       <c r="E33" s="3" t="s">
@@ -1765,7 +3453,7 @@
       <c r="G33" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H33" s="17"/>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="2:8" ht="32" customHeight="1">
       <c r="B34" s="10" t="s">
@@ -1774,19 +3462,19 @@
       <c r="C34" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="17" t="s">
         <v>62</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H34" s="17"/>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="2:8" ht="32" customHeight="1">
       <c r="B35" s="14" t="s">
@@ -1795,7 +3483,7 @@
       <c r="C35" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E35" s="3" t="s">
@@ -1807,7 +3495,7 @@
       <c r="G35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H35" s="17"/>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="2:8" ht="32" customHeight="1">
       <c r="B36" s="12" t="s">
@@ -1816,19 +3504,19 @@
       <c r="C36" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="17" t="s">
         <v>66</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="H36" s="17"/>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="2:8" ht="32" customHeight="1">
       <c r="B37" s="7" t="s">
@@ -1837,19 +3525,19 @@
       <c r="C37" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="16" t="s">
         <v>68</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="20" t="s">
         <v>135</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H37" s="17"/>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="2:8" ht="32" customHeight="1">
       <c r="B38" s="13" t="s">
@@ -1858,7 +3546,7 @@
       <c r="C38" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E38" s="8" t="s">
@@ -1870,7 +3558,7 @@
       <c r="G38" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H38" s="17"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="2:8" ht="32" customHeight="1">
       <c r="B39" s="14" t="s">
@@ -1879,7 +3567,7 @@
       <c r="C39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="16" t="s">
         <v>58</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1891,7 +3579,7 @@
       <c r="G39" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H39" s="17"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="2:8" ht="32" customHeight="1">
       <c r="B40" s="13" t="s">
@@ -1900,7 +3588,7 @@
       <c r="C40" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="17" t="s">
         <v>73</v>
       </c>
       <c r="E40" s="8" t="s">
@@ -1912,7 +3600,7 @@
       <c r="G40" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="H40" s="17"/>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="2:8" ht="32" customHeight="1">
       <c r="B41" s="14" t="s">
@@ -1921,7 +3609,7 @@
       <c r="C41" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="16" t="s">
         <v>75</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1933,7 +3621,7 @@
       <c r="G41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H41" s="17"/>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="2:8" ht="32" customHeight="1">
       <c r="B42" s="12" t="s">
@@ -1942,19 +3630,19 @@
       <c r="C42" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="17" t="s">
         <v>77</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="21" t="s">
         <v>135</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H42" s="17"/>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="2:8" ht="32" customHeight="1">
       <c r="B43" s="14" t="s">
@@ -1963,11 +3651,11 @@
       <c r="C43" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="16" t="s">
         <v>79</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F43" s="20">
         <v>4.1666666666666664E-2</v>
@@ -1975,7 +3663,7 @@
       <c r="G43" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H43" s="17"/>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="2:8" ht="32" customHeight="1">
       <c r="B44" s="13" t="s">
@@ -1984,11 +3672,11 @@
       <c r="C44" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="19" t="s">
+      <c r="D44" s="17" t="s">
         <v>81</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F44" s="21">
         <v>0.54166666666666663</v>
@@ -1996,7 +3684,7 @@
       <c r="G44" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H44" s="17"/>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="2:8" ht="32" customHeight="1">
       <c r="B45" s="14" t="s">
@@ -2005,7 +3693,7 @@
       <c r="C45" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="16" t="s">
         <v>83</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -2017,12 +3705,12 @@
       <c r="G45" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H45" s="17"/>
+      <c r="H45" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="44" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>